<commit_message>
attribute plots and code+excel update
</commit_message>
<xml_diff>
--- a/Data/Prostate.xlsx
+++ b/Data/Prostate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g46435\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greta\Documents\GitHub\ML_fall2018\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{90F03F0E-FE0D-4321-86C5-22898ED6BE15}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A9FB38-E744-4AEA-B5FA-19721534F4BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{D48C4C1C-04C2-4D9D-A047-E241E7EA7095}"/>
   </bookViews>
@@ -27,31 +27,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="13">
   <si>
-    <t>lcavol</t>
-  </si>
-  <si>
-    <t>lweight</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>lbph</t>
-  </si>
-  <si>
-    <t>svi</t>
-  </si>
-  <si>
-    <t>lcp</t>
-  </si>
-  <si>
-    <t>gleason</t>
-  </si>
-  <si>
     <t>pgg45</t>
-  </si>
-  <si>
-    <t>lpsa</t>
   </si>
   <si>
     <t>train</t>
@@ -65,12 +41,36 @@
   <si>
     <t>ID</t>
   </si>
+  <si>
+    <t>lCaVol</t>
+  </si>
+  <si>
+    <t>lWeight</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>lBPH</t>
+  </si>
+  <si>
+    <t>SVI</t>
+  </si>
+  <si>
+    <t>lCP</t>
+  </si>
+  <si>
+    <t>Gleason</t>
+  </si>
+  <si>
+    <t>lPSA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -426,48 +426,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3AC5FF-EE3E-4542-A24C-638C4B82D254}">
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="K1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -499,10 +499,10 @@
         <v>-0.43078290000000002</v>
       </c>
       <c r="K2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -534,10 +534,10 @@
         <v>-0.16251889999999999</v>
       </c>
       <c r="K3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -569,10 +569,10 @@
         <v>-0.16251889999999999</v>
       </c>
       <c r="K4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -604,10 +604,10 @@
         <v>-0.16251889999999999</v>
       </c>
       <c r="K5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -639,10 +639,10 @@
         <v>0.37156359999999999</v>
       </c>
       <c r="K6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -674,10 +674,10 @@
         <v>0.76546780000000003</v>
       </c>
       <c r="K7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -709,10 +709,10 @@
         <v>0.76546780000000003</v>
       </c>
       <c r="K8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -744,10 +744,10 @@
         <v>0.85441529999999999</v>
       </c>
       <c r="K9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -779,10 +779,10 @@
         <v>1.0473189999999999</v>
       </c>
       <c r="K10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -814,10 +814,10 @@
         <v>1.0473189999999999</v>
       </c>
       <c r="K11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -849,10 +849,10 @@
         <v>1.2669476</v>
       </c>
       <c r="K12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -884,10 +884,10 @@
         <v>1.2669476</v>
       </c>
       <c r="K13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -919,10 +919,10 @@
         <v>1.2669476</v>
       </c>
       <c r="K14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -954,10 +954,10 @@
         <v>1.3480730999999999</v>
       </c>
       <c r="K15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -989,10 +989,10 @@
         <v>1.3987168999999999</v>
       </c>
       <c r="K16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1024,10 +1024,10 @@
         <v>1.4469190000000001</v>
       </c>
       <c r="K17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1059,10 +1059,10 @@
         <v>1.4701758</v>
       </c>
       <c r="K18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1094,10 +1094,10 @@
         <v>1.4929041000000001</v>
       </c>
       <c r="K19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1129,10 +1129,10 @@
         <v>1.5581446000000001</v>
       </c>
       <c r="K20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1164,10 +1164,10 @@
         <v>1.5993876</v>
       </c>
       <c r="K21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1199,10 +1199,10 @@
         <v>1.6389967000000001</v>
       </c>
       <c r="K22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1234,10 +1234,10 @@
         <v>1.6582281000000001</v>
       </c>
       <c r="K23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1269,10 +1269,10 @@
         <v>1.6956156</v>
       </c>
       <c r="K24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1304,10 +1304,10 @@
         <v>1.7137979000000001</v>
       </c>
       <c r="K25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1339,10 +1339,10 @@
         <v>1.7316555</v>
       </c>
       <c r="K26" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1374,10 +1374,10 @@
         <v>1.7664416999999999</v>
       </c>
       <c r="K27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1409,10 +1409,10 @@
         <v>1.8000582999999999</v>
       </c>
       <c r="K28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1444,10 +1444,10 @@
         <v>1.8164521</v>
       </c>
       <c r="K29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1479,10 +1479,10 @@
         <v>1.8484548000000001</v>
       </c>
       <c r="K30" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1514,10 +1514,10 @@
         <v>1.8946168999999999</v>
       </c>
       <c r="K31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1549,10 +1549,10 @@
         <v>1.9242486999999999</v>
       </c>
       <c r="K32" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1584,10 +1584,10 @@
         <v>2.0082140000000002</v>
       </c>
       <c r="K33" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1619,10 +1619,10 @@
         <v>2.0082140000000002</v>
       </c>
       <c r="K34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1654,10 +1654,10 @@
         <v>2.0215475999999999</v>
       </c>
       <c r="K35" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1689,10 +1689,10 @@
         <v>2.0476928000000001</v>
       </c>
       <c r="K36" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1724,10 +1724,10 @@
         <v>2.0856721</v>
       </c>
       <c r="K37" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1759,10 +1759,10 @@
         <v>2.1575593</v>
       </c>
       <c r="K38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1794,10 +1794,10 @@
         <v>2.1916535000000001</v>
       </c>
       <c r="K39" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1829,10 +1829,10 @@
         <v>2.2137538999999999</v>
       </c>
       <c r="K40" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1864,10 +1864,10 @@
         <v>2.2772673000000001</v>
       </c>
       <c r="K41" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1899,10 +1899,10 @@
         <v>2.2975726000000001</v>
       </c>
       <c r="K42" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1934,10 +1934,10 @@
         <v>2.3075725999999999</v>
       </c>
       <c r="K43" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1969,10 +1969,10 @@
         <v>2.3272776999999998</v>
       </c>
       <c r="K44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2004,10 +2004,10 @@
         <v>2.3749058000000001</v>
       </c>
       <c r="K45" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2039,10 +2039,10 @@
         <v>2.5217206000000001</v>
       </c>
       <c r="K46" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2074,10 +2074,10 @@
         <v>2.5533437999999999</v>
       </c>
       <c r="K47" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2109,10 +2109,10 @@
         <v>2.5687880999999999</v>
       </c>
       <c r="K48" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2144,10 +2144,10 @@
         <v>2.5687880999999999</v>
       </c>
       <c r="K49" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2179,10 +2179,10 @@
         <v>2.5915164000000002</v>
       </c>
       <c r="K50" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2214,10 +2214,10 @@
         <v>2.5915164000000002</v>
       </c>
       <c r="K51" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2249,10 +2249,10 @@
         <v>2.6567569</v>
       </c>
       <c r="K52" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2284,10 +2284,10 @@
         <v>2.6775910000000001</v>
       </c>
       <c r="K53" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -2319,10 +2319,10 @@
         <v>2.6844402999999999</v>
       </c>
       <c r="K54" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -2354,10 +2354,10 @@
         <v>2.6912430999999999</v>
       </c>
       <c r="K55" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -2389,10 +2389,10 @@
         <v>2.7047113</v>
       </c>
       <c r="K56" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -2424,10 +2424,10 @@
         <v>2.7180005</v>
       </c>
       <c r="K57" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -2459,10 +2459,10 @@
         <v>2.7880929000000001</v>
       </c>
       <c r="K58" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -2494,10 +2494,10 @@
         <v>2.7942279000000001</v>
       </c>
       <c r="K59" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -2529,10 +2529,10 @@
         <v>2.8063861000000001</v>
       </c>
       <c r="K60" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -2564,10 +2564,10 @@
         <v>2.8124102</v>
       </c>
       <c r="K61" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -2599,10 +2599,10 @@
         <v>2.8419981999999999</v>
       </c>
       <c r="K62" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -2634,10 +2634,10 @@
         <v>2.8535925</v>
       </c>
       <c r="K63" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -2669,10 +2669,10 @@
         <v>2.8535925</v>
       </c>
       <c r="K64" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -2704,10 +2704,10 @@
         <v>2.8820035000000002</v>
       </c>
       <c r="K65" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -2739,10 +2739,10 @@
         <v>2.8820035000000002</v>
       </c>
       <c r="K66" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -2774,10 +2774,10 @@
         <v>2.8875901000000002</v>
       </c>
       <c r="K67" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -2809,10 +2809,10 @@
         <v>2.9204697999999998</v>
       </c>
       <c r="K68" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -2844,10 +2844,10 @@
         <v>2.9626923999999999</v>
       </c>
       <c r="K69" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -2879,10 +2879,10 @@
         <v>2.9626923999999999</v>
       </c>
       <c r="K70" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -2914,10 +2914,10 @@
         <v>2.9729752999999999</v>
       </c>
       <c r="K71" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -2949,10 +2949,10 @@
         <v>3.0130808999999998</v>
       </c>
       <c r="K72" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -2984,10 +2984,10 @@
         <v>3.0373538999999998</v>
       </c>
       <c r="K73" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -3019,10 +3019,10 @@
         <v>3.0563568999999999</v>
       </c>
       <c r="K74" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -3054,10 +3054,10 @@
         <v>3.0750055000000001</v>
       </c>
       <c r="K75" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -3089,10 +3089,10 @@
         <v>3.2752561999999998</v>
       </c>
       <c r="K76" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -3124,10 +3124,10 @@
         <v>3.3375474000000001</v>
       </c>
       <c r="K77" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -3159,10 +3159,10 @@
         <v>3.3928291000000002</v>
       </c>
       <c r="K78" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -3194,10 +3194,10 @@
         <v>3.4355988000000002</v>
       </c>
       <c r="K79" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -3229,10 +3229,10 @@
         <v>3.4578926999999999</v>
       </c>
       <c r="K80" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -3264,10 +3264,10 @@
         <v>3.5130368999999999</v>
       </c>
       <c r="K81" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -3299,10 +3299,10 @@
         <v>3.5160130999999999</v>
       </c>
       <c r="K82" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -3334,10 +3334,10 @@
         <v>3.5307626000000001</v>
       </c>
       <c r="K83" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -3369,10 +3369,10 @@
         <v>3.5652984000000001</v>
       </c>
       <c r="K84" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -3404,10 +3404,10 @@
         <v>3.5709401999999999</v>
       </c>
       <c r="K85" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -3439,10 +3439,10 @@
         <v>3.5876768999999999</v>
       </c>
       <c r="K86" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -3474,10 +3474,10 @@
         <v>3.6309855</v>
       </c>
       <c r="K87" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -3509,10 +3509,10 @@
         <v>3.6800909000000002</v>
       </c>
       <c r="K88" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -3544,10 +3544,10 @@
         <v>3.7123518</v>
       </c>
       <c r="K89" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -3579,10 +3579,10 @@
         <v>3.9843437000000002</v>
       </c>
       <c r="K90" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -3614,10 +3614,10 @@
         <v>3.9936029999999998</v>
       </c>
       <c r="K91" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -3649,10 +3649,10 @@
         <v>4.0298059999999998</v>
       </c>
       <c r="K92" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -3684,10 +3684,10 @@
         <v>4.1295507999999996</v>
       </c>
       <c r="K93" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -3719,10 +3719,10 @@
         <v>4.3851468000000002</v>
       </c>
       <c r="K94" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -3754,10 +3754,10 @@
         <v>4.6844434000000001</v>
       </c>
       <c r="K95" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -3789,10 +3789,10 @@
         <v>5.1431244999999999</v>
       </c>
       <c r="K96" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -3824,10 +3824,10 @@
         <v>5.4775090000000004</v>
       </c>
       <c r="K97" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -3859,7 +3859,7 @@
         <v>5.5829322000000001</v>
       </c>
       <c r="K98" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>